<commit_message>
Added spin-wheel in page and updated spreadsheet code.
</commit_message>
<xml_diff>
--- a/resources/template_output.xlsx
+++ b/resources/template_output.xlsx
@@ -5,23 +5,28 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1033" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="1075" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="1078" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="1035" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="1178" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="1135" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="1003" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -113,26 +118,78 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -145,59 +202,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -223,7 +228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>